<commit_message>
added code for ELK integration
</commit_message>
<xml_diff>
--- a/src/test/resources/testexcel/testdata.xlsx
+++ b/src/test/resources/testexcel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>username</t>
   </si>
@@ -92,9 +92,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Test whether I can drive my test from excel</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Test Case 2</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -149,25 +143,40 @@
     <t>somethingElse</t>
   </si>
   <si>
-    <t>Test whether the description is displayed properly in extent report</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>sjdknf</t>
   </si>
   <si>
     <t>bhsd</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>jsf</t>
   </si>
   <si>
     <t>jkf</t>
+  </si>
+  <si>
+    <t>To check whether the user can sort the apple laptops</t>
+  </si>
+  <si>
+    <t>testcase3</t>
+  </si>
+  <si>
+    <t>sjdnc</t>
+  </si>
+  <si>
+    <t>sdjn</t>
+  </si>
+  <si>
+    <t>jkb</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>Test Case 3</t>
   </si>
 </sst>
 </file>
@@ -510,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -525,19 +534,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -545,10 +554,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>24</v>
@@ -562,16 +571,16 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -579,33 +588,50 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -615,19 +641,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.08984375" customWidth="1"/>
+    <col min="2" max="3" width="15.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -635,166 +661,216 @@
         <v>23</v>
       </c>
       <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="F9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="E11" t="s">
         <v>49</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F11" t="s">
         <v>50</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>